<commit_message>
Added Arduino Watch design and schematics, made minor improvements to AFNT App, updated logs and completed Design Chapter
</commit_message>
<xml_diff>
--- a/Documents/Test Sheet.xlsx
+++ b/Documents/Test Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14970486-72D1-4EA1-A923-62D3B61DCF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{14970486-72D1-4EA1-A923-62D3B61DCF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC6E8F8-770C-44DA-A66C-B219E226014C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3630" windowWidth="19200" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -640,26 +640,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -687,6 +672,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -766,751 +758,14 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1855,7 +1110,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,6 +1196,9 @@
       <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
       <c r="I3" s="6" t="s">
         <v>90</v>
       </c>
@@ -1975,6 +1233,9 @@
       <c r="G4" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
       <c r="I4" s="6" t="s">
         <v>91</v>
       </c>
@@ -2267,7 +1528,7 @@
       <c r="M15" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="3" t="s">
         <v>149</v>
       </c>
       <c r="O15" s="4" t="s">
@@ -2372,7 +1633,7 @@
       <c r="M20" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="3" t="s">
         <v>155</v>
       </c>
       <c r="O20" s="4" t="s">
@@ -2720,87 +1981,87 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1 A2:C2">
-    <cfRule type="endsWith" dxfId="47" priority="9" operator="endsWith" text="Not Implemented">
+    <cfRule type="endsWith" dxfId="23" priority="9" operator="endsWith" text="Not Implemented">
       <formula>RIGHT(A1,LEN("Not Implemented"))="Not Implemented"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="10" operator="beginsWith" text="Partically Functional">
+    <cfRule type="beginsWith" dxfId="22" priority="10" operator="beginsWith" text="Partically Functional">
       <formula>LEFT(A1,LEN("Partically Functional"))="Partically Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="45" priority="11" operator="beginsWith" text="Not Functional">
+    <cfRule type="beginsWith" dxfId="21" priority="11" operator="beginsWith" text="Not Functional">
       <formula>LEFT(A1,LEN("Not Functional"))="Not Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="44" priority="12" operator="beginsWith" text="Functional">
+    <cfRule type="beginsWith" dxfId="20" priority="12" operator="beginsWith" text="Functional">
       <formula>LEFT(A1,LEN("Functional"))="Functional"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="endsWith" dxfId="19" priority="1" operator="endsWith" text="Not Implemented">
+      <formula>RIGHT(A1,LEN("Not Implemented"))="Not Implemented"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="2" operator="beginsWith" text="Partically Functional">
+      <formula>LEFT(A1,LEN("Partically Functional"))="Partically Functional"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="3" operator="beginsWith" text="Not Functional">
+      <formula>LEFT(A1,LEN("Not Functional"))="Not Functional"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="4" operator="beginsWith" text="Functional">
+      <formula>LEFT(A1,LEN("Functional"))="Functional"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="15" priority="23" operator="beginsWith" text="Partially Functional">
+      <formula>LEFT(A1,LEN("Partially Functional"))="Partially Functional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1 E2:G304 J4:K4 I4:I5">
-    <cfRule type="endsWith" dxfId="43" priority="21" operator="endsWith" text="Not Implemented">
+    <cfRule type="endsWith" dxfId="14" priority="21" operator="endsWith" text="Not Implemented">
       <formula>RIGHT(E1,LEN("Not Implemented"))="Not Implemented"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="24" operator="beginsWith" text="Not Functional">
+    <cfRule type="beginsWith" dxfId="13" priority="24" operator="beginsWith" text="Not Functional">
       <formula>LEFT(E1,LEN("Not Functional"))="Not Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="25" operator="beginsWith" text="Functional">
+    <cfRule type="beginsWith" dxfId="12" priority="25" operator="beginsWith" text="Functional">
       <formula>LEFT(E1,LEN("Functional"))="Functional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1 I2:K3">
-    <cfRule type="endsWith" dxfId="40" priority="17" operator="endsWith" text="Not Implemented">
+    <cfRule type="endsWith" dxfId="11" priority="17" operator="endsWith" text="Not Implemented">
       <formula>RIGHT(I1,LEN("Not Implemented"))="Not Implemented"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="18" operator="beginsWith" text="Partically Functional">
+    <cfRule type="beginsWith" dxfId="10" priority="18" operator="beginsWith" text="Partically Functional">
       <formula>LEFT(I1,LEN("Partically Functional"))="Partically Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="38" priority="19" operator="beginsWith" text="Not Functional">
+    <cfRule type="beginsWith" dxfId="9" priority="19" operator="beginsWith" text="Not Functional">
       <formula>LEFT(I1,LEN("Not Functional"))="Not Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="20" operator="beginsWith" text="Functional">
+    <cfRule type="beginsWith" dxfId="8" priority="20" operator="beginsWith" text="Functional">
       <formula>LEFT(I1,LEN("Functional"))="Functional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1 M2:O2">
-    <cfRule type="endsWith" dxfId="36" priority="13" operator="endsWith" text="Not Implemented">
+    <cfRule type="endsWith" dxfId="7" priority="13" operator="endsWith" text="Not Implemented">
       <formula>RIGHT(M1,LEN("Not Implemented"))="Not Implemented"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="35" priority="14" operator="beginsWith" text="Partically Functional">
+    <cfRule type="beginsWith" dxfId="6" priority="14" operator="beginsWith" text="Partically Functional">
       <formula>LEFT(M1,LEN("Partically Functional"))="Partically Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="15" operator="beginsWith" text="Not Functional">
+    <cfRule type="beginsWith" dxfId="5" priority="15" operator="beginsWith" text="Not Functional">
       <formula>LEFT(M1,LEN("Not Functional"))="Not Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="16" operator="beginsWith" text="Functional">
+    <cfRule type="beginsWith" dxfId="4" priority="16" operator="beginsWith" text="Functional">
       <formula>LEFT(M1,LEN("Functional"))="Functional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O16">
-    <cfRule type="endsWith" dxfId="32" priority="5" operator="endsWith" text="Not Implemented">
+    <cfRule type="endsWith" dxfId="3" priority="5" operator="endsWith" text="Not Implemented">
       <formula>RIGHT(O3,LEN("Not Implemented"))="Not Implemented"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="6" operator="beginsWith" text="Partically Functional">
+    <cfRule type="beginsWith" dxfId="2" priority="6" operator="beginsWith" text="Partically Functional">
       <formula>LEFT(O3,LEN("Partically Functional"))="Partically Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="7" operator="beginsWith" text="Not Functional">
+    <cfRule type="beginsWith" dxfId="1" priority="7" operator="beginsWith" text="Not Functional">
       <formula>LEFT(O3,LEN("Not Functional"))="Not Functional"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="29" priority="8" operator="beginsWith" text="Functional">
+    <cfRule type="beginsWith" dxfId="0" priority="8" operator="beginsWith" text="Functional">
       <formula>LEFT(O3,LEN("Functional"))="Functional"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="beginsWith" dxfId="28" priority="23" operator="beginsWith" text="Partially Functional">
-      <formula>LEFT(A1,LEN("Partially Functional"))="Partially Functional"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="27" priority="1" operator="endsWith" text="Not Implemented">
-      <formula>RIGHT(A1,LEN("Not Implemented"))="Not Implemented"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="2" operator="beginsWith" text="Partically Functional">
-      <formula>LEFT(A1,LEN("Partically Functional"))="Partically Functional"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="3" operator="beginsWith" text="Not Functional">
-      <formula>LEFT(A1,LEN("Not Functional"))="Not Functional"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="4" operator="beginsWith" text="Functional">
-      <formula>LEFT(A1,LEN("Functional"))="Functional"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>